<commit_message>
Diverse veranderingen eind 2025
</commit_message>
<xml_diff>
--- a/icon helper.xlsx
+++ b/icon helper.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f7f4011b2811a15/Documenten/Arduino/BKOS4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1509" documentId="8_{E71812E1-E4B2-4A16-BF5D-1EED3CB7A1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D4F2AB3-A085-4B67-BFCE-CEC46C5C1ACF}"/>
+  <xr:revisionPtr revIDLastSave="1515" documentId="8_{E71812E1-E4B2-4A16-BF5D-1EED3CB7A1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48EA57C6-7445-423F-B32C-E8D5867E423B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB644C52-5EB8-4C3F-91B4-A03DCFFD6266}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EB644C52-5EB8-4C3F-91B4-A03DCFFD6266}"/>
   </bookViews>
   <sheets>
     <sheet name="30" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -459,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30FD981-21C0-46E6-A80E-F0D6C2605ECA}">
   <dimension ref="B1:EL255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ153" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="EJ161" sqref="EJ161"/>
+    <sheetView topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BX171" sqref="BX171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13796,11 +13797,11 @@
         <v>12</v>
       </c>
       <c r="CZ163">
-        <f t="shared" ref="CZ163:CZ176" si="50">CC163</f>
+        <f t="shared" ref="CZ163:CZ172" si="50">CC163</f>
         <v>9</v>
       </c>
       <c r="DA163">
-        <f t="shared" ref="DA163:DA176" si="51">CD163</f>
+        <f t="shared" ref="DA163:DA172" si="51">CD163</f>
         <v>0</v>
       </c>
       <c r="DJ163">
@@ -14103,11 +14104,11 @@
         <v>5,4,21,0</v>
       </c>
       <c r="CA165">
-        <f t="shared" ref="CA165:CA191" si="56">BE165+BF165</f>
+        <f t="shared" ref="CA165:CA189" si="56">BE165+BF165</f>
         <v>9</v>
       </c>
       <c r="CB165">
-        <f t="shared" ref="CB165:CB191" si="57">AI165-BF165</f>
+        <f t="shared" ref="CB165:CB189" si="57">AI165-BF165</f>
         <v>16</v>
       </c>
       <c r="CC165">
@@ -17316,7 +17317,7 @@
         <v>10</v>
       </c>
       <c r="BG183">
-        <f t="shared" ref="BG183:BG191" si="67">30-BE183-BF183</f>
+        <f t="shared" ref="BG183:BG189" si="67">30-BE183-BF183</f>
         <v>18</v>
       </c>
       <c r="BH183">
@@ -20689,4 +20690,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BD4EF3-C59D-43C6-B1C0-6599BBBB7F73}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>37.5</v>
+      </c>
+      <c r="B1">
+        <f>A1/2</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <f>A2/2</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <f>B1-B2</f>
+        <v>10.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
260114b: Voorbereidingen gemaakt voor een swicht tussen versie 4 en 5 en daarmee een handmatige update knop.
</commit_message>
<xml_diff>
--- a/icon helper.xlsx
+++ b/icon helper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f7f4011b2811a15/Documenten/Arduino/BKOS4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3360" documentId="8_{E71812E1-E4B2-4A16-BF5D-1EED3CB7A1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAB1EB9D-0DF0-4583-B126-81BEF25C1AC2}"/>
+  <xr:revisionPtr revIDLastSave="3527" documentId="8_{E71812E1-E4B2-4A16-BF5D-1EED3CB7A1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F5A1A7C-F728-467B-AC58-C4F5C8C560BE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-195" windowWidth="29040" windowHeight="15720" xr2:uid="{EB644C52-5EB8-4C3F-91B4-A03DCFFD6266}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB644C52-5EB8-4C3F-91B4-A03DCFFD6266}"/>
   </bookViews>
   <sheets>
     <sheet name="30" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="11">
   <si>
     <t>W</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30FD981-21C0-46E6-A80E-F0D6C2605ECA}">
-  <dimension ref="B1:EL386"/>
+  <dimension ref="B1:EL418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BT356" sqref="BT356"/>
+    <sheetView tabSelected="1" topLeftCell="A376" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AW388" sqref="AW388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28220,7 +28220,7 @@
         <v>0</v>
       </c>
       <c r="AT325">
-        <f t="shared" ref="AT325:AT353" si="81">SUM(AH325:AR325)</f>
+        <f t="shared" ref="AT325:AT326" si="81">SUM(AH325:AR325)</f>
         <v>30</v>
       </c>
       <c r="AW325" t="str">
@@ -30608,7 +30608,7 @@
         <v>5,20,5,0</v>
       </c>
       <c r="BE360">
-        <f t="shared" ref="BE360:BE366" si="96">BE359-2</f>
+        <f t="shared" ref="BE360" si="96">BE359-2</f>
         <v>5</v>
       </c>
       <c r="BF360">
@@ -31478,7 +31478,7 @@
         <v>2,26,2,0</v>
       </c>
       <c r="BE365">
-        <f t="shared" ref="BE365:BE368" si="99">BE363-1</f>
+        <f t="shared" ref="BE365:BE367" si="99">BE363-1</f>
         <v>2</v>
       </c>
       <c r="BF365">
@@ -31683,11 +31683,11 @@
         <v>19</v>
       </c>
       <c r="CB366">
-        <f t="shared" ref="CB366:CB368" si="101">CB365+1</f>
+        <f t="shared" ref="CB366:CB367" si="101">CB365+1</f>
         <v>10</v>
       </c>
       <c r="CC366">
-        <f t="shared" ref="CC366:CC368" si="102">CC364-1</f>
+        <f t="shared" ref="CC366:CC367" si="102">CC364-1</f>
         <v>1</v>
       </c>
       <c r="CD366">
@@ -32196,7 +32196,7 @@
         <v>17</v>
       </c>
       <c r="CB369">
-        <f t="shared" ref="CB369:CB375" si="103">30-CA369</f>
+        <f t="shared" ref="CB369:CB374" si="103">30-CA369</f>
         <v>13</v>
       </c>
       <c r="CM369">
@@ -33810,7 +33810,7 @@
         <v>16</v>
       </c>
       <c r="CC379">
-        <f t="shared" ref="CC379:CC384" si="106">CC377+1</f>
+        <f t="shared" ref="CC379:CC382" si="106">CC377+1</f>
         <v>2</v>
       </c>
       <c r="CD379">
@@ -34411,7 +34411,7 @@
         <v>5,20,5,0</v>
       </c>
       <c r="BE383">
-        <f t="shared" ref="BE383:BE384" si="108">BE382+1</f>
+        <f t="shared" ref="BE383" si="108">BE382+1</f>
         <v>5</v>
       </c>
       <c r="BF383">
@@ -34858,8 +34858,2013 @@
         <v>30,0</v>
       </c>
     </row>
+    <row r="388" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="AH388" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI388" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ388" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK388" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL388" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM388" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW388" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,AW389:AW418)</f>
+        <v>15,1,14,0,14,1,1,1,13,0,13,1,3,1,12,0,12,1,5,1,11,0,11,1,7,1,10,0,10,1,9,1,9,0,9,1,11,1,8,0,8,1,13,1,7,0,7,1,15,1,6,0,6,1,17,1,5,0,5,1,19,1,4,0,4,1,21,1,3,0,3,1,23,1,2,0,2,7,13,7,1,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,1,13,1,7,0,8,15,7,0,30,0,30,0,8,15,7,0,30,0,30,0,8,15,7,0,30,0</v>
+      </c>
+    </row>
+    <row r="389" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B389" s="1"/>
+      <c r="C389" s="1"/>
+      <c r="D389" s="1"/>
+      <c r="E389" s="1"/>
+      <c r="F389" s="1"/>
+      <c r="G389" s="1"/>
+      <c r="H389" s="1"/>
+      <c r="I389" s="1"/>
+      <c r="J389" s="1"/>
+      <c r="K389" s="1"/>
+      <c r="L389" s="1"/>
+      <c r="M389" s="1"/>
+      <c r="N389" s="1"/>
+      <c r="O389" s="1"/>
+      <c r="P389" s="1"/>
+      <c r="Q389" s="1">
+        <v>1</v>
+      </c>
+      <c r="R389" s="1"/>
+      <c r="S389" s="1"/>
+      <c r="T389" s="1"/>
+      <c r="U389" s="1"/>
+      <c r="V389" s="1"/>
+      <c r="W389" s="1"/>
+      <c r="X389" s="1"/>
+      <c r="Y389" s="1"/>
+      <c r="Z389" s="1"/>
+      <c r="AA389" s="1"/>
+      <c r="AB389" s="1"/>
+      <c r="AC389" s="1"/>
+      <c r="AD389" s="1"/>
+      <c r="AE389" s="1"/>
+      <c r="AH389">
+        <v>15</v>
+      </c>
+      <c r="AI389">
+        <v>1</v>
+      </c>
+      <c r="AJ389">
+        <v>14</v>
+      </c>
+      <c r="AK389">
+        <v>0</v>
+      </c>
+      <c r="AT389">
+        <f>SUM(AH389:AR389)</f>
+        <v>30</v>
+      </c>
+      <c r="AW389" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,AH389:AS389)</f>
+        <v>15,1,14,0</v>
+      </c>
+    </row>
+    <row r="390" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B390" s="1"/>
+      <c r="C390" s="1"/>
+      <c r="D390" s="1"/>
+      <c r="E390" s="1"/>
+      <c r="F390" s="1"/>
+      <c r="G390" s="1"/>
+      <c r="H390" s="1"/>
+      <c r="I390" s="1"/>
+      <c r="J390" s="1"/>
+      <c r="K390" s="1"/>
+      <c r="L390" s="1"/>
+      <c r="M390" s="1"/>
+      <c r="N390" s="1"/>
+      <c r="O390" s="1"/>
+      <c r="P390" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q390" s="1"/>
+      <c r="R390" s="1">
+        <v>1</v>
+      </c>
+      <c r="S390" s="1"/>
+      <c r="T390" s="1"/>
+      <c r="U390" s="1"/>
+      <c r="V390" s="1"/>
+      <c r="W390" s="1"/>
+      <c r="X390" s="1"/>
+      <c r="Y390" s="1"/>
+      <c r="Z390" s="1"/>
+      <c r="AA390" s="1"/>
+      <c r="AB390" s="1"/>
+      <c r="AC390" s="1"/>
+      <c r="AD390" s="1"/>
+      <c r="AE390" s="1"/>
+      <c r="AH390">
+        <v>14</v>
+      </c>
+      <c r="AI390">
+        <v>1</v>
+      </c>
+      <c r="AJ390">
+        <v>1</v>
+      </c>
+      <c r="AK390">
+        <v>1</v>
+      </c>
+      <c r="AL390">
+        <v>13</v>
+      </c>
+      <c r="AM390">
+        <v>0</v>
+      </c>
+      <c r="AT390">
+        <f t="shared" ref="AT390:AT418" si="110">SUM(AH390:AR390)</f>
+        <v>30</v>
+      </c>
+      <c r="AW390" t="str">
+        <f t="shared" ref="AW390:AW418" si="111">_xlfn.TEXTJOIN(",",TRUE,AH390:AS390)</f>
+        <v>14,1,1,1,13,0</v>
+      </c>
+    </row>
+    <row r="391" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B391" s="1"/>
+      <c r="C391" s="1"/>
+      <c r="D391" s="1"/>
+      <c r="E391" s="1"/>
+      <c r="F391" s="1"/>
+      <c r="G391" s="1"/>
+      <c r="H391" s="1"/>
+      <c r="I391" s="1"/>
+      <c r="J391" s="1"/>
+      <c r="K391" s="1"/>
+      <c r="L391" s="1"/>
+      <c r="M391" s="1"/>
+      <c r="N391" s="1"/>
+      <c r="O391" s="1">
+        <v>1</v>
+      </c>
+      <c r="P391" s="1"/>
+      <c r="Q391" s="1"/>
+      <c r="R391" s="1"/>
+      <c r="S391" s="1">
+        <v>1</v>
+      </c>
+      <c r="T391" s="1"/>
+      <c r="U391" s="1"/>
+      <c r="V391" s="1"/>
+      <c r="W391" s="1"/>
+      <c r="X391" s="1"/>
+      <c r="Y391" s="1"/>
+      <c r="Z391" s="1"/>
+      <c r="AA391" s="1"/>
+      <c r="AB391" s="1"/>
+      <c r="AC391" s="1"/>
+      <c r="AD391" s="1"/>
+      <c r="AE391" s="1"/>
+      <c r="AH391">
+        <f>AH390-1</f>
+        <v>13</v>
+      </c>
+      <c r="AI391">
+        <f>AI390</f>
+        <v>1</v>
+      </c>
+      <c r="AJ391">
+        <f>AJ390+2</f>
+        <v>3</v>
+      </c>
+      <c r="AK391">
+        <f>AK390</f>
+        <v>1</v>
+      </c>
+      <c r="AL391">
+        <f>AL390-1</f>
+        <v>12</v>
+      </c>
+      <c r="AM391">
+        <f>AM390</f>
+        <v>0</v>
+      </c>
+      <c r="AT391">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW391" t="str">
+        <f t="shared" si="111"/>
+        <v>13,1,3,1,12,0</v>
+      </c>
+    </row>
+    <row r="392" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B392" s="1"/>
+      <c r="C392" s="1"/>
+      <c r="D392" s="1"/>
+      <c r="E392" s="1"/>
+      <c r="F392" s="1"/>
+      <c r="G392" s="1"/>
+      <c r="H392" s="1"/>
+      <c r="I392" s="1"/>
+      <c r="J392" s="1"/>
+      <c r="K392" s="1"/>
+      <c r="L392" s="1"/>
+      <c r="M392" s="1"/>
+      <c r="N392" s="1">
+        <v>1</v>
+      </c>
+      <c r="O392" s="1"/>
+      <c r="P392" s="1"/>
+      <c r="Q392" s="1"/>
+      <c r="R392" s="1"/>
+      <c r="S392" s="1"/>
+      <c r="T392" s="1">
+        <v>1</v>
+      </c>
+      <c r="U392" s="1"/>
+      <c r="V392" s="1"/>
+      <c r="W392" s="1"/>
+      <c r="X392" s="1"/>
+      <c r="Y392" s="1"/>
+      <c r="Z392" s="1"/>
+      <c r="AA392" s="1"/>
+      <c r="AB392" s="1"/>
+      <c r="AC392" s="1"/>
+      <c r="AD392" s="1"/>
+      <c r="AE392" s="1"/>
+      <c r="AH392">
+        <f t="shared" ref="AH392:AH402" si="112">AH391-1</f>
+        <v>12</v>
+      </c>
+      <c r="AI392">
+        <f t="shared" ref="AI392:AI402" si="113">AI391</f>
+        <v>1</v>
+      </c>
+      <c r="AJ392">
+        <f t="shared" ref="AJ392:AJ402" si="114">AJ391+2</f>
+        <v>5</v>
+      </c>
+      <c r="AK392">
+        <f t="shared" ref="AK392:AK402" si="115">AK391</f>
+        <v>1</v>
+      </c>
+      <c r="AL392">
+        <f t="shared" ref="AL392:AL402" si="116">AL391-1</f>
+        <v>11</v>
+      </c>
+      <c r="AM392">
+        <f t="shared" ref="AM392:AM402" si="117">AM391</f>
+        <v>0</v>
+      </c>
+      <c r="AT392">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW392" t="str">
+        <f t="shared" si="111"/>
+        <v>12,1,5,1,11,0</v>
+      </c>
+    </row>
+    <row r="393" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B393" s="1"/>
+      <c r="C393" s="1"/>
+      <c r="D393" s="1"/>
+      <c r="E393" s="1"/>
+      <c r="F393" s="1"/>
+      <c r="G393" s="1"/>
+      <c r="H393" s="1"/>
+      <c r="I393" s="1"/>
+      <c r="J393" s="1"/>
+      <c r="K393" s="1"/>
+      <c r="L393" s="1"/>
+      <c r="M393" s="1">
+        <v>1</v>
+      </c>
+      <c r="N393" s="1"/>
+      <c r="O393" s="1"/>
+      <c r="P393" s="1"/>
+      <c r="Q393" s="1"/>
+      <c r="R393" s="1"/>
+      <c r="S393" s="1"/>
+      <c r="T393" s="1"/>
+      <c r="U393" s="1">
+        <v>1</v>
+      </c>
+      <c r="V393" s="1"/>
+      <c r="W393" s="1"/>
+      <c r="X393" s="1"/>
+      <c r="Y393" s="1"/>
+      <c r="Z393" s="1"/>
+      <c r="AA393" s="1"/>
+      <c r="AB393" s="1"/>
+      <c r="AC393" s="1"/>
+      <c r="AD393" s="1"/>
+      <c r="AE393" s="1"/>
+      <c r="AH393">
+        <f t="shared" si="112"/>
+        <v>11</v>
+      </c>
+      <c r="AI393">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ393">
+        <f t="shared" si="114"/>
+        <v>7</v>
+      </c>
+      <c r="AK393">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL393">
+        <f t="shared" si="116"/>
+        <v>10</v>
+      </c>
+      <c r="AM393">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT393">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW393" t="str">
+        <f t="shared" si="111"/>
+        <v>11,1,7,1,10,0</v>
+      </c>
+    </row>
+    <row r="394" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B394" s="1"/>
+      <c r="C394" s="1"/>
+      <c r="D394" s="1"/>
+      <c r="E394" s="1"/>
+      <c r="F394" s="1"/>
+      <c r="G394" s="1"/>
+      <c r="H394" s="1"/>
+      <c r="I394" s="1"/>
+      <c r="J394" s="1"/>
+      <c r="K394" s="1"/>
+      <c r="L394" s="1">
+        <v>1</v>
+      </c>
+      <c r="M394" s="1"/>
+      <c r="N394" s="1"/>
+      <c r="O394" s="1"/>
+      <c r="P394" s="1"/>
+      <c r="Q394" s="1"/>
+      <c r="R394" s="1"/>
+      <c r="S394" s="1"/>
+      <c r="T394" s="1"/>
+      <c r="U394" s="1"/>
+      <c r="V394" s="1">
+        <v>1</v>
+      </c>
+      <c r="W394" s="1"/>
+      <c r="X394" s="1"/>
+      <c r="Y394" s="1"/>
+      <c r="Z394" s="1"/>
+      <c r="AA394" s="1"/>
+      <c r="AB394" s="1"/>
+      <c r="AC394" s="1"/>
+      <c r="AD394" s="1"/>
+      <c r="AE394" s="1"/>
+      <c r="AH394">
+        <f t="shared" si="112"/>
+        <v>10</v>
+      </c>
+      <c r="AI394">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ394">
+        <f t="shared" si="114"/>
+        <v>9</v>
+      </c>
+      <c r="AK394">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL394">
+        <f t="shared" si="116"/>
+        <v>9</v>
+      </c>
+      <c r="AM394">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT394">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW394" t="str">
+        <f t="shared" si="111"/>
+        <v>10,1,9,1,9,0</v>
+      </c>
+    </row>
+    <row r="395" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B395" s="1"/>
+      <c r="C395" s="1"/>
+      <c r="D395" s="1"/>
+      <c r="E395" s="1"/>
+      <c r="F395" s="1"/>
+      <c r="G395" s="1"/>
+      <c r="H395" s="1"/>
+      <c r="I395" s="1"/>
+      <c r="J395" s="1"/>
+      <c r="K395" s="1">
+        <v>1</v>
+      </c>
+      <c r="L395" s="1"/>
+      <c r="M395" s="1"/>
+      <c r="N395" s="1"/>
+      <c r="O395" s="1"/>
+      <c r="P395" s="1"/>
+      <c r="Q395" s="1"/>
+      <c r="R395" s="1"/>
+      <c r="S395" s="1"/>
+      <c r="T395" s="1"/>
+      <c r="U395" s="1"/>
+      <c r="V395" s="1"/>
+      <c r="W395" s="1">
+        <v>1</v>
+      </c>
+      <c r="X395" s="1"/>
+      <c r="Y395" s="1"/>
+      <c r="Z395" s="1"/>
+      <c r="AA395" s="1"/>
+      <c r="AB395" s="1"/>
+      <c r="AC395" s="1"/>
+      <c r="AD395" s="1"/>
+      <c r="AE395" s="1"/>
+      <c r="AH395">
+        <f t="shared" si="112"/>
+        <v>9</v>
+      </c>
+      <c r="AI395">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ395">
+        <f t="shared" si="114"/>
+        <v>11</v>
+      </c>
+      <c r="AK395">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL395">
+        <f t="shared" si="116"/>
+        <v>8</v>
+      </c>
+      <c r="AM395">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT395">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW395" t="str">
+        <f t="shared" si="111"/>
+        <v>9,1,11,1,8,0</v>
+      </c>
+    </row>
+    <row r="396" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B396" s="1"/>
+      <c r="C396" s="1"/>
+      <c r="D396" s="1"/>
+      <c r="E396" s="1"/>
+      <c r="F396" s="1"/>
+      <c r="G396" s="1"/>
+      <c r="H396" s="1"/>
+      <c r="I396" s="1"/>
+      <c r="J396" s="1">
+        <v>1</v>
+      </c>
+      <c r="K396" s="1"/>
+      <c r="L396" s="1"/>
+      <c r="M396" s="1"/>
+      <c r="N396" s="1"/>
+      <c r="O396" s="1"/>
+      <c r="P396" s="1"/>
+      <c r="Q396" s="1"/>
+      <c r="R396" s="1"/>
+      <c r="S396" s="1"/>
+      <c r="T396" s="1"/>
+      <c r="U396" s="1"/>
+      <c r="V396" s="1"/>
+      <c r="W396" s="1"/>
+      <c r="X396" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y396" s="1"/>
+      <c r="Z396" s="1"/>
+      <c r="AA396" s="1"/>
+      <c r="AB396" s="1"/>
+      <c r="AC396" s="1"/>
+      <c r="AD396" s="1"/>
+      <c r="AE396" s="1"/>
+      <c r="AH396">
+        <f t="shared" si="112"/>
+        <v>8</v>
+      </c>
+      <c r="AI396">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ396">
+        <f t="shared" si="114"/>
+        <v>13</v>
+      </c>
+      <c r="AK396">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL396">
+        <f t="shared" si="116"/>
+        <v>7</v>
+      </c>
+      <c r="AM396">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT396">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW396" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="397" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B397" s="1"/>
+      <c r="C397" s="1"/>
+      <c r="D397" s="1"/>
+      <c r="E397" s="1"/>
+      <c r="F397" s="1"/>
+      <c r="G397" s="1"/>
+      <c r="H397" s="1"/>
+      <c r="I397" s="1">
+        <v>1</v>
+      </c>
+      <c r="J397" s="1"/>
+      <c r="K397" s="1"/>
+      <c r="L397" s="1"/>
+      <c r="M397" s="1"/>
+      <c r="N397" s="1"/>
+      <c r="O397" s="1"/>
+      <c r="P397" s="1"/>
+      <c r="Q397" s="1"/>
+      <c r="R397" s="1"/>
+      <c r="S397" s="1"/>
+      <c r="T397" s="1"/>
+      <c r="U397" s="1"/>
+      <c r="V397" s="1"/>
+      <c r="W397" s="1"/>
+      <c r="X397" s="1"/>
+      <c r="Y397" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z397" s="1"/>
+      <c r="AA397" s="1"/>
+      <c r="AB397" s="1"/>
+      <c r="AC397" s="1"/>
+      <c r="AD397" s="1"/>
+      <c r="AE397" s="1"/>
+      <c r="AH397">
+        <f t="shared" si="112"/>
+        <v>7</v>
+      </c>
+      <c r="AI397">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ397">
+        <f t="shared" si="114"/>
+        <v>15</v>
+      </c>
+      <c r="AK397">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL397">
+        <f t="shared" si="116"/>
+        <v>6</v>
+      </c>
+      <c r="AM397">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT397">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW397" t="str">
+        <f t="shared" si="111"/>
+        <v>7,1,15,1,6,0</v>
+      </c>
+    </row>
+    <row r="398" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B398" s="1"/>
+      <c r="C398" s="1"/>
+      <c r="D398" s="1"/>
+      <c r="E398" s="1"/>
+      <c r="F398" s="1"/>
+      <c r="G398" s="1"/>
+      <c r="H398" s="1">
+        <v>1</v>
+      </c>
+      <c r="I398" s="1"/>
+      <c r="J398" s="1"/>
+      <c r="K398" s="1"/>
+      <c r="L398" s="1"/>
+      <c r="M398" s="1"/>
+      <c r="N398" s="1"/>
+      <c r="O398" s="1"/>
+      <c r="P398" s="1"/>
+      <c r="Q398" s="1"/>
+      <c r="R398" s="1"/>
+      <c r="S398" s="1"/>
+      <c r="T398" s="1"/>
+      <c r="U398" s="1"/>
+      <c r="V398" s="1"/>
+      <c r="W398" s="1"/>
+      <c r="X398" s="1"/>
+      <c r="Y398" s="1"/>
+      <c r="Z398" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA398" s="1"/>
+      <c r="AB398" s="1"/>
+      <c r="AC398" s="1"/>
+      <c r="AD398" s="1"/>
+      <c r="AE398" s="1"/>
+      <c r="AH398">
+        <f t="shared" si="112"/>
+        <v>6</v>
+      </c>
+      <c r="AI398">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ398">
+        <f t="shared" si="114"/>
+        <v>17</v>
+      </c>
+      <c r="AK398">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL398">
+        <f t="shared" si="116"/>
+        <v>5</v>
+      </c>
+      <c r="AM398">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT398">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW398" t="str">
+        <f t="shared" si="111"/>
+        <v>6,1,17,1,5,0</v>
+      </c>
+    </row>
+    <row r="399" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B399" s="1"/>
+      <c r="C399" s="1"/>
+      <c r="D399" s="1"/>
+      <c r="E399" s="1"/>
+      <c r="F399" s="1"/>
+      <c r="G399" s="1">
+        <v>1</v>
+      </c>
+      <c r="H399" s="1"/>
+      <c r="I399" s="1"/>
+      <c r="J399" s="1"/>
+      <c r="K399" s="1"/>
+      <c r="L399" s="1"/>
+      <c r="M399" s="1"/>
+      <c r="N399" s="1"/>
+      <c r="O399" s="1"/>
+      <c r="P399" s="1"/>
+      <c r="Q399" s="1"/>
+      <c r="R399" s="1"/>
+      <c r="S399" s="1"/>
+      <c r="T399" s="1"/>
+      <c r="U399" s="1"/>
+      <c r="V399" s="1"/>
+      <c r="W399" s="1"/>
+      <c r="X399" s="1"/>
+      <c r="Y399" s="1"/>
+      <c r="Z399" s="1"/>
+      <c r="AA399" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB399" s="1"/>
+      <c r="AC399" s="1"/>
+      <c r="AD399" s="1"/>
+      <c r="AE399" s="1"/>
+      <c r="AH399">
+        <f t="shared" si="112"/>
+        <v>5</v>
+      </c>
+      <c r="AI399">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ399">
+        <f t="shared" si="114"/>
+        <v>19</v>
+      </c>
+      <c r="AK399">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL399">
+        <f t="shared" si="116"/>
+        <v>4</v>
+      </c>
+      <c r="AM399">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT399">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW399" t="str">
+        <f t="shared" si="111"/>
+        <v>5,1,19,1,4,0</v>
+      </c>
+    </row>
+    <row r="400" spans="2:117" x14ac:dyDescent="0.25">
+      <c r="B400" s="1"/>
+      <c r="C400" s="1"/>
+      <c r="D400" s="1"/>
+      <c r="E400" s="1"/>
+      <c r="F400" s="1">
+        <v>1</v>
+      </c>
+      <c r="G400" s="1"/>
+      <c r="H400" s="1"/>
+      <c r="I400" s="1"/>
+      <c r="J400" s="1"/>
+      <c r="K400" s="1"/>
+      <c r="L400" s="1"/>
+      <c r="M400" s="1"/>
+      <c r="N400" s="1"/>
+      <c r="O400" s="1"/>
+      <c r="P400" s="1"/>
+      <c r="Q400" s="1"/>
+      <c r="R400" s="1"/>
+      <c r="S400" s="1"/>
+      <c r="T400" s="1"/>
+      <c r="U400" s="1"/>
+      <c r="V400" s="1"/>
+      <c r="W400" s="1"/>
+      <c r="X400" s="1"/>
+      <c r="Y400" s="1"/>
+      <c r="Z400" s="1"/>
+      <c r="AA400" s="1"/>
+      <c r="AB400" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC400" s="1"/>
+      <c r="AD400" s="1"/>
+      <c r="AE400" s="1"/>
+      <c r="AH400">
+        <f t="shared" si="112"/>
+        <v>4</v>
+      </c>
+      <c r="AI400">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ400">
+        <f t="shared" si="114"/>
+        <v>21</v>
+      </c>
+      <c r="AK400">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL400">
+        <f t="shared" si="116"/>
+        <v>3</v>
+      </c>
+      <c r="AM400">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT400">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW400" t="str">
+        <f t="shared" si="111"/>
+        <v>4,1,21,1,3,0</v>
+      </c>
+    </row>
+    <row r="401" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B401" s="1"/>
+      <c r="C401" s="1"/>
+      <c r="D401" s="1"/>
+      <c r="E401" s="1">
+        <v>1</v>
+      </c>
+      <c r="F401" s="1"/>
+      <c r="G401" s="1"/>
+      <c r="H401" s="1"/>
+      <c r="I401" s="1"/>
+      <c r="J401" s="1"/>
+      <c r="K401" s="1"/>
+      <c r="L401" s="1"/>
+      <c r="M401" s="1"/>
+      <c r="N401" s="1"/>
+      <c r="O401" s="1"/>
+      <c r="P401" s="1"/>
+      <c r="Q401" s="1"/>
+      <c r="R401" s="1"/>
+      <c r="S401" s="1"/>
+      <c r="T401" s="1"/>
+      <c r="U401" s="1"/>
+      <c r="V401" s="1"/>
+      <c r="W401" s="1"/>
+      <c r="X401" s="1"/>
+      <c r="Y401" s="1"/>
+      <c r="Z401" s="1"/>
+      <c r="AA401" s="1"/>
+      <c r="AB401" s="1"/>
+      <c r="AC401" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD401" s="1"/>
+      <c r="AE401" s="1"/>
+      <c r="AH401">
+        <f t="shared" si="112"/>
+        <v>3</v>
+      </c>
+      <c r="AI401">
+        <f t="shared" si="113"/>
+        <v>1</v>
+      </c>
+      <c r="AJ401">
+        <f t="shared" si="114"/>
+        <v>23</v>
+      </c>
+      <c r="AK401">
+        <f t="shared" si="115"/>
+        <v>1</v>
+      </c>
+      <c r="AL401">
+        <f t="shared" si="116"/>
+        <v>2</v>
+      </c>
+      <c r="AM401">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT401">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW401" t="str">
+        <f t="shared" si="111"/>
+        <v>3,1,23,1,2,0</v>
+      </c>
+    </row>
+    <row r="402" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B402" s="1"/>
+      <c r="C402" s="1"/>
+      <c r="D402" s="1">
+        <v>1</v>
+      </c>
+      <c r="E402" s="1">
+        <v>1</v>
+      </c>
+      <c r="F402" s="1">
+        <v>1</v>
+      </c>
+      <c r="G402" s="1">
+        <v>1</v>
+      </c>
+      <c r="H402" s="1">
+        <v>1</v>
+      </c>
+      <c r="I402" s="1">
+        <v>1</v>
+      </c>
+      <c r="J402" s="1">
+        <v>1</v>
+      </c>
+      <c r="K402" s="1"/>
+      <c r="L402" s="1"/>
+      <c r="M402" s="1"/>
+      <c r="N402" s="1"/>
+      <c r="O402" s="1"/>
+      <c r="P402" s="1"/>
+      <c r="Q402" s="1"/>
+      <c r="R402" s="1"/>
+      <c r="S402" s="1"/>
+      <c r="T402" s="1"/>
+      <c r="U402" s="1"/>
+      <c r="V402" s="1"/>
+      <c r="W402" s="1"/>
+      <c r="X402" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y402" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD402" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE402" s="1"/>
+      <c r="AH402">
+        <f t="shared" si="112"/>
+        <v>2</v>
+      </c>
+      <c r="AI402">
+        <v>7</v>
+      </c>
+      <c r="AJ402">
+        <v>13</v>
+      </c>
+      <c r="AK402">
+        <v>7</v>
+      </c>
+      <c r="AL402">
+        <f t="shared" si="116"/>
+        <v>1</v>
+      </c>
+      <c r="AM402">
+        <f t="shared" si="117"/>
+        <v>0</v>
+      </c>
+      <c r="AT402">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW402" t="str">
+        <f t="shared" si="111"/>
+        <v>2,7,13,7,1,0</v>
+      </c>
+    </row>
+    <row r="403" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B403" s="1"/>
+      <c r="C403" s="1"/>
+      <c r="D403" s="1"/>
+      <c r="E403" s="1"/>
+      <c r="F403" s="1"/>
+      <c r="G403" s="1"/>
+      <c r="H403" s="1"/>
+      <c r="I403" s="1"/>
+      <c r="J403" s="1">
+        <v>1</v>
+      </c>
+      <c r="K403" s="1"/>
+      <c r="L403" s="1"/>
+      <c r="M403" s="1"/>
+      <c r="N403" s="1"/>
+      <c r="O403" s="1"/>
+      <c r="P403" s="1"/>
+      <c r="Q403" s="1"/>
+      <c r="R403" s="1"/>
+      <c r="S403" s="1"/>
+      <c r="T403" s="1"/>
+      <c r="U403" s="1"/>
+      <c r="V403" s="1"/>
+      <c r="W403" s="1"/>
+      <c r="X403" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y403" s="1"/>
+      <c r="Z403" s="1"/>
+      <c r="AA403" s="1"/>
+      <c r="AB403" s="1"/>
+      <c r="AC403" s="1"/>
+      <c r="AD403" s="1"/>
+      <c r="AE403" s="1"/>
+      <c r="AH403">
+        <v>8</v>
+      </c>
+      <c r="AI403">
+        <v>1</v>
+      </c>
+      <c r="AJ403">
+        <v>13</v>
+      </c>
+      <c r="AK403">
+        <v>1</v>
+      </c>
+      <c r="AL403">
+        <v>7</v>
+      </c>
+      <c r="AM403">
+        <v>0</v>
+      </c>
+      <c r="AT403">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW403" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="404" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B404" s="1"/>
+      <c r="C404" s="1"/>
+      <c r="D404" s="1"/>
+      <c r="E404" s="1"/>
+      <c r="F404" s="1"/>
+      <c r="G404" s="1"/>
+      <c r="H404" s="1"/>
+      <c r="I404" s="1"/>
+      <c r="J404" s="1">
+        <v>1</v>
+      </c>
+      <c r="K404" s="1"/>
+      <c r="L404" s="1"/>
+      <c r="M404" s="1"/>
+      <c r="N404" s="1"/>
+      <c r="O404" s="1"/>
+      <c r="P404" s="1"/>
+      <c r="Q404" s="1"/>
+      <c r="R404" s="1"/>
+      <c r="S404" s="1"/>
+      <c r="T404" s="1"/>
+      <c r="U404" s="1"/>
+      <c r="V404" s="1"/>
+      <c r="W404" s="1"/>
+      <c r="X404" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y404" s="1"/>
+      <c r="Z404" s="1"/>
+      <c r="AA404" s="1"/>
+      <c r="AB404" s="1"/>
+      <c r="AC404" s="1"/>
+      <c r="AD404" s="1"/>
+      <c r="AE404" s="1"/>
+      <c r="AH404">
+        <f>AH403</f>
+        <v>8</v>
+      </c>
+      <c r="AI404">
+        <f t="shared" ref="AI404:AM404" si="118">AI403</f>
+        <v>1</v>
+      </c>
+      <c r="AJ404">
+        <f t="shared" si="118"/>
+        <v>13</v>
+      </c>
+      <c r="AK404">
+        <f t="shared" si="118"/>
+        <v>1</v>
+      </c>
+      <c r="AL404">
+        <f t="shared" si="118"/>
+        <v>7</v>
+      </c>
+      <c r="AM404">
+        <f t="shared" si="118"/>
+        <v>0</v>
+      </c>
+      <c r="AT404">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW404" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="405" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B405" s="1"/>
+      <c r="C405" s="1"/>
+      <c r="D405" s="1"/>
+      <c r="E405" s="1"/>
+      <c r="F405" s="1"/>
+      <c r="G405" s="1"/>
+      <c r="H405" s="1"/>
+      <c r="I405" s="1"/>
+      <c r="J405" s="1">
+        <v>1</v>
+      </c>
+      <c r="K405" s="1"/>
+      <c r="L405" s="1"/>
+      <c r="M405" s="1"/>
+      <c r="N405" s="1"/>
+      <c r="O405" s="1"/>
+      <c r="P405" s="1"/>
+      <c r="Q405" s="1"/>
+      <c r="R405" s="1"/>
+      <c r="S405" s="1"/>
+      <c r="T405" s="1"/>
+      <c r="U405" s="1"/>
+      <c r="V405" s="1"/>
+      <c r="W405" s="1"/>
+      <c r="X405" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y405" s="1"/>
+      <c r="Z405" s="1"/>
+      <c r="AA405" s="1"/>
+      <c r="AB405" s="1"/>
+      <c r="AC405" s="1"/>
+      <c r="AD405" s="1"/>
+      <c r="AE405" s="1"/>
+      <c r="AH405">
+        <f t="shared" ref="AH405:AH410" si="119">AH404</f>
+        <v>8</v>
+      </c>
+      <c r="AI405">
+        <f t="shared" ref="AI405:AI410" si="120">AI404</f>
+        <v>1</v>
+      </c>
+      <c r="AJ405">
+        <f t="shared" ref="AJ405:AJ410" si="121">AJ404</f>
+        <v>13</v>
+      </c>
+      <c r="AK405">
+        <f t="shared" ref="AK405:AK410" si="122">AK404</f>
+        <v>1</v>
+      </c>
+      <c r="AL405">
+        <f t="shared" ref="AL405:AL410" si="123">AL404</f>
+        <v>7</v>
+      </c>
+      <c r="AM405">
+        <f t="shared" ref="AM405:AM410" si="124">AM404</f>
+        <v>0</v>
+      </c>
+      <c r="AT405">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW405" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="406" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B406" s="1"/>
+      <c r="C406" s="1"/>
+      <c r="D406" s="1"/>
+      <c r="E406" s="1"/>
+      <c r="F406" s="1"/>
+      <c r="G406" s="1"/>
+      <c r="H406" s="1"/>
+      <c r="I406" s="1"/>
+      <c r="J406" s="1">
+        <v>1</v>
+      </c>
+      <c r="K406" s="1"/>
+      <c r="L406" s="1"/>
+      <c r="M406" s="1"/>
+      <c r="N406" s="1"/>
+      <c r="O406" s="1"/>
+      <c r="P406" s="1"/>
+      <c r="Q406" s="1"/>
+      <c r="R406" s="1"/>
+      <c r="S406" s="1"/>
+      <c r="T406" s="1"/>
+      <c r="U406" s="1"/>
+      <c r="V406" s="1"/>
+      <c r="W406" s="1"/>
+      <c r="X406" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y406" s="1"/>
+      <c r="Z406" s="1"/>
+      <c r="AA406" s="1"/>
+      <c r="AB406" s="1"/>
+      <c r="AC406" s="1"/>
+      <c r="AD406" s="1"/>
+      <c r="AE406" s="1"/>
+      <c r="AH406">
+        <f t="shared" si="119"/>
+        <v>8</v>
+      </c>
+      <c r="AI406">
+        <f t="shared" si="120"/>
+        <v>1</v>
+      </c>
+      <c r="AJ406">
+        <f t="shared" si="121"/>
+        <v>13</v>
+      </c>
+      <c r="AK406">
+        <f t="shared" si="122"/>
+        <v>1</v>
+      </c>
+      <c r="AL406">
+        <f t="shared" si="123"/>
+        <v>7</v>
+      </c>
+      <c r="AM406">
+        <f t="shared" si="124"/>
+        <v>0</v>
+      </c>
+      <c r="AT406">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW406" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="407" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B407" s="1"/>
+      <c r="C407" s="1"/>
+      <c r="D407" s="1"/>
+      <c r="E407" s="1"/>
+      <c r="F407" s="1"/>
+      <c r="G407" s="1"/>
+      <c r="H407" s="1"/>
+      <c r="I407" s="1"/>
+      <c r="J407" s="1">
+        <v>1</v>
+      </c>
+      <c r="K407" s="1"/>
+      <c r="L407" s="1"/>
+      <c r="M407" s="1"/>
+      <c r="N407" s="1"/>
+      <c r="O407" s="1"/>
+      <c r="P407" s="1"/>
+      <c r="Q407" s="1"/>
+      <c r="R407" s="1"/>
+      <c r="S407" s="1"/>
+      <c r="T407" s="1"/>
+      <c r="U407" s="1"/>
+      <c r="V407" s="1"/>
+      <c r="W407" s="1"/>
+      <c r="X407" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y407" s="1"/>
+      <c r="Z407" s="1"/>
+      <c r="AA407" s="1"/>
+      <c r="AB407" s="1"/>
+      <c r="AC407" s="1"/>
+      <c r="AD407" s="1"/>
+      <c r="AE407" s="1"/>
+      <c r="AH407">
+        <f t="shared" si="119"/>
+        <v>8</v>
+      </c>
+      <c r="AI407">
+        <f t="shared" si="120"/>
+        <v>1</v>
+      </c>
+      <c r="AJ407">
+        <f t="shared" si="121"/>
+        <v>13</v>
+      </c>
+      <c r="AK407">
+        <f t="shared" si="122"/>
+        <v>1</v>
+      </c>
+      <c r="AL407">
+        <f t="shared" si="123"/>
+        <v>7</v>
+      </c>
+      <c r="AM407">
+        <f t="shared" si="124"/>
+        <v>0</v>
+      </c>
+      <c r="AT407">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW407" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="408" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B408" s="1"/>
+      <c r="C408" s="1"/>
+      <c r="D408" s="1"/>
+      <c r="E408" s="1"/>
+      <c r="F408" s="1"/>
+      <c r="G408" s="1"/>
+      <c r="H408" s="1"/>
+      <c r="I408" s="1"/>
+      <c r="J408" s="1">
+        <v>1</v>
+      </c>
+      <c r="K408" s="1"/>
+      <c r="L408" s="1"/>
+      <c r="M408" s="1"/>
+      <c r="N408" s="1"/>
+      <c r="O408" s="1"/>
+      <c r="P408" s="1"/>
+      <c r="Q408" s="1"/>
+      <c r="R408" s="1"/>
+      <c r="S408" s="1"/>
+      <c r="T408" s="1"/>
+      <c r="U408" s="1"/>
+      <c r="V408" s="1"/>
+      <c r="W408" s="1"/>
+      <c r="X408" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y408" s="1"/>
+      <c r="Z408" s="1"/>
+      <c r="AA408" s="1"/>
+      <c r="AB408" s="1"/>
+      <c r="AC408" s="1"/>
+      <c r="AD408" s="1"/>
+      <c r="AE408" s="1"/>
+      <c r="AH408">
+        <f t="shared" si="119"/>
+        <v>8</v>
+      </c>
+      <c r="AI408">
+        <f t="shared" si="120"/>
+        <v>1</v>
+      </c>
+      <c r="AJ408">
+        <f t="shared" si="121"/>
+        <v>13</v>
+      </c>
+      <c r="AK408">
+        <f t="shared" si="122"/>
+        <v>1</v>
+      </c>
+      <c r="AL408">
+        <f t="shared" si="123"/>
+        <v>7</v>
+      </c>
+      <c r="AM408">
+        <f t="shared" si="124"/>
+        <v>0</v>
+      </c>
+      <c r="AT408">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW408" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="409" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B409" s="1"/>
+      <c r="C409" s="1"/>
+      <c r="D409" s="1"/>
+      <c r="E409" s="1"/>
+      <c r="F409" s="1"/>
+      <c r="G409" s="1"/>
+      <c r="H409" s="1"/>
+      <c r="I409" s="1"/>
+      <c r="J409" s="1">
+        <v>1</v>
+      </c>
+      <c r="K409" s="1"/>
+      <c r="L409" s="1"/>
+      <c r="M409" s="1"/>
+      <c r="N409" s="1"/>
+      <c r="O409" s="1"/>
+      <c r="P409" s="1"/>
+      <c r="Q409" s="1"/>
+      <c r="R409" s="1"/>
+      <c r="S409" s="1"/>
+      <c r="T409" s="1"/>
+      <c r="U409" s="1"/>
+      <c r="V409" s="1"/>
+      <c r="W409" s="1"/>
+      <c r="X409" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y409" s="1"/>
+      <c r="Z409" s="1"/>
+      <c r="AA409" s="1"/>
+      <c r="AB409" s="1"/>
+      <c r="AC409" s="1"/>
+      <c r="AD409" s="1"/>
+      <c r="AE409" s="1"/>
+      <c r="AH409">
+        <f t="shared" si="119"/>
+        <v>8</v>
+      </c>
+      <c r="AI409">
+        <f t="shared" si="120"/>
+        <v>1</v>
+      </c>
+      <c r="AJ409">
+        <f t="shared" si="121"/>
+        <v>13</v>
+      </c>
+      <c r="AK409">
+        <f t="shared" si="122"/>
+        <v>1</v>
+      </c>
+      <c r="AL409">
+        <f t="shared" si="123"/>
+        <v>7</v>
+      </c>
+      <c r="AM409">
+        <f t="shared" si="124"/>
+        <v>0</v>
+      </c>
+      <c r="AT409">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW409" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="410" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B410" s="1"/>
+      <c r="C410" s="1"/>
+      <c r="D410" s="1"/>
+      <c r="E410" s="1"/>
+      <c r="F410" s="1"/>
+      <c r="G410" s="1"/>
+      <c r="H410" s="1"/>
+      <c r="I410" s="1"/>
+      <c r="J410" s="1">
+        <v>1</v>
+      </c>
+      <c r="K410" s="1"/>
+      <c r="L410" s="1"/>
+      <c r="M410" s="1"/>
+      <c r="N410" s="1"/>
+      <c r="O410" s="1"/>
+      <c r="P410" s="1"/>
+      <c r="Q410" s="1"/>
+      <c r="R410" s="1"/>
+      <c r="S410" s="1"/>
+      <c r="T410" s="1"/>
+      <c r="U410" s="1"/>
+      <c r="V410" s="1"/>
+      <c r="W410" s="1"/>
+      <c r="X410" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y410" s="1"/>
+      <c r="Z410" s="1"/>
+      <c r="AA410" s="1"/>
+      <c r="AB410" s="1"/>
+      <c r="AC410" s="1"/>
+      <c r="AD410" s="1"/>
+      <c r="AE410" s="1"/>
+      <c r="AH410">
+        <f t="shared" si="119"/>
+        <v>8</v>
+      </c>
+      <c r="AI410">
+        <f t="shared" si="120"/>
+        <v>1</v>
+      </c>
+      <c r="AJ410">
+        <f t="shared" si="121"/>
+        <v>13</v>
+      </c>
+      <c r="AK410">
+        <f t="shared" si="122"/>
+        <v>1</v>
+      </c>
+      <c r="AL410">
+        <f t="shared" si="123"/>
+        <v>7</v>
+      </c>
+      <c r="AM410">
+        <f t="shared" si="124"/>
+        <v>0</v>
+      </c>
+      <c r="AT410">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW410" t="str">
+        <f t="shared" si="111"/>
+        <v>8,1,13,1,7,0</v>
+      </c>
+    </row>
+    <row r="411" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B411" s="1"/>
+      <c r="C411" s="1"/>
+      <c r="D411" s="1"/>
+      <c r="E411" s="1"/>
+      <c r="F411" s="1"/>
+      <c r="G411" s="1"/>
+      <c r="H411" s="1"/>
+      <c r="I411" s="1"/>
+      <c r="J411" s="1">
+        <v>1</v>
+      </c>
+      <c r="K411" s="1">
+        <v>1</v>
+      </c>
+      <c r="L411" s="1">
+        <v>1</v>
+      </c>
+      <c r="M411" s="1">
+        <v>1</v>
+      </c>
+      <c r="N411" s="1">
+        <v>1</v>
+      </c>
+      <c r="O411" s="1">
+        <v>1</v>
+      </c>
+      <c r="P411" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q411" s="1">
+        <v>1</v>
+      </c>
+      <c r="R411" s="1">
+        <v>1</v>
+      </c>
+      <c r="S411" s="1">
+        <v>1</v>
+      </c>
+      <c r="T411" s="1">
+        <v>1</v>
+      </c>
+      <c r="U411" s="1">
+        <v>1</v>
+      </c>
+      <c r="V411" s="1">
+        <v>1</v>
+      </c>
+      <c r="W411" s="1">
+        <v>1</v>
+      </c>
+      <c r="X411" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y411" s="1"/>
+      <c r="Z411" s="1"/>
+      <c r="AA411" s="1"/>
+      <c r="AB411" s="1"/>
+      <c r="AC411" s="1"/>
+      <c r="AD411" s="1"/>
+      <c r="AE411" s="1"/>
+      <c r="AH411">
+        <v>8</v>
+      </c>
+      <c r="AI411">
+        <v>15</v>
+      </c>
+      <c r="AJ411">
+        <v>7</v>
+      </c>
+      <c r="AK411">
+        <v>0</v>
+      </c>
+      <c r="AT411">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW411" t="str">
+        <f t="shared" si="111"/>
+        <v>8,15,7,0</v>
+      </c>
+    </row>
+    <row r="412" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B412" s="1"/>
+      <c r="C412" s="1"/>
+      <c r="D412" s="1"/>
+      <c r="E412" s="1"/>
+      <c r="F412" s="1"/>
+      <c r="G412" s="1"/>
+      <c r="H412" s="1"/>
+      <c r="I412" s="1"/>
+      <c r="J412" s="1"/>
+      <c r="K412" s="1"/>
+      <c r="L412" s="1"/>
+      <c r="M412" s="1"/>
+      <c r="N412" s="1"/>
+      <c r="O412" s="1"/>
+      <c r="P412" s="1"/>
+      <c r="Q412" s="1"/>
+      <c r="R412" s="1"/>
+      <c r="S412" s="1"/>
+      <c r="T412" s="1"/>
+      <c r="U412" s="1"/>
+      <c r="V412" s="1"/>
+      <c r="W412" s="1"/>
+      <c r="X412" s="1"/>
+      <c r="Y412" s="1"/>
+      <c r="Z412" s="1"/>
+      <c r="AA412" s="1"/>
+      <c r="AB412" s="1"/>
+      <c r="AC412" s="1"/>
+      <c r="AD412" s="1"/>
+      <c r="AE412" s="1"/>
+      <c r="AH412">
+        <v>30</v>
+      </c>
+      <c r="AI412">
+        <v>0</v>
+      </c>
+      <c r="AT412">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW412" t="str">
+        <f t="shared" si="111"/>
+        <v>30,0</v>
+      </c>
+    </row>
+    <row r="413" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B413" s="1"/>
+      <c r="C413" s="1"/>
+      <c r="D413" s="1"/>
+      <c r="E413" s="1"/>
+      <c r="F413" s="1"/>
+      <c r="G413" s="1"/>
+      <c r="H413" s="1"/>
+      <c r="I413" s="1"/>
+      <c r="J413" s="1"/>
+      <c r="K413" s="1"/>
+      <c r="L413" s="1"/>
+      <c r="M413" s="1"/>
+      <c r="N413" s="1"/>
+      <c r="O413" s="1"/>
+      <c r="P413" s="1"/>
+      <c r="Q413" s="1"/>
+      <c r="R413" s="1"/>
+      <c r="S413" s="1"/>
+      <c r="T413" s="1"/>
+      <c r="U413" s="1"/>
+      <c r="V413" s="1"/>
+      <c r="W413" s="1"/>
+      <c r="X413" s="1"/>
+      <c r="Y413" s="1"/>
+      <c r="Z413" s="1"/>
+      <c r="AA413" s="1"/>
+      <c r="AB413" s="1"/>
+      <c r="AC413" s="1"/>
+      <c r="AD413" s="1"/>
+      <c r="AE413" s="1"/>
+      <c r="AH413">
+        <v>30</v>
+      </c>
+      <c r="AI413">
+        <v>0</v>
+      </c>
+      <c r="AT413">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW413" t="str">
+        <f t="shared" si="111"/>
+        <v>30,0</v>
+      </c>
+    </row>
+    <row r="414" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B414" s="1"/>
+      <c r="C414" s="1"/>
+      <c r="D414" s="1"/>
+      <c r="E414" s="1"/>
+      <c r="F414" s="1"/>
+      <c r="G414" s="1"/>
+      <c r="H414" s="1"/>
+      <c r="I414" s="1"/>
+      <c r="J414" s="1">
+        <v>1</v>
+      </c>
+      <c r="K414" s="1">
+        <v>1</v>
+      </c>
+      <c r="L414" s="1">
+        <v>1</v>
+      </c>
+      <c r="M414" s="1">
+        <v>1</v>
+      </c>
+      <c r="N414" s="1">
+        <v>1</v>
+      </c>
+      <c r="O414" s="1">
+        <v>1</v>
+      </c>
+      <c r="P414" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q414" s="1">
+        <v>1</v>
+      </c>
+      <c r="R414" s="1">
+        <v>1</v>
+      </c>
+      <c r="S414" s="1">
+        <v>1</v>
+      </c>
+      <c r="T414" s="1">
+        <v>1</v>
+      </c>
+      <c r="U414" s="1">
+        <v>1</v>
+      </c>
+      <c r="V414" s="1">
+        <v>1</v>
+      </c>
+      <c r="W414" s="1">
+        <v>1</v>
+      </c>
+      <c r="X414" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y414" s="1"/>
+      <c r="Z414" s="1"/>
+      <c r="AA414" s="1"/>
+      <c r="AB414" s="1"/>
+      <c r="AC414" s="1"/>
+      <c r="AD414" s="1"/>
+      <c r="AE414" s="1"/>
+      <c r="AH414">
+        <f>AH411</f>
+        <v>8</v>
+      </c>
+      <c r="AI414">
+        <f t="shared" ref="AI414:AK414" si="125">AI411</f>
+        <v>15</v>
+      </c>
+      <c r="AJ414">
+        <f t="shared" si="125"/>
+        <v>7</v>
+      </c>
+      <c r="AK414">
+        <f t="shared" si="125"/>
+        <v>0</v>
+      </c>
+      <c r="AT414">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW414" t="str">
+        <f t="shared" si="111"/>
+        <v>8,15,7,0</v>
+      </c>
+    </row>
+    <row r="415" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B415" s="1"/>
+      <c r="C415" s="1"/>
+      <c r="D415" s="1"/>
+      <c r="E415" s="1"/>
+      <c r="F415" s="1"/>
+      <c r="G415" s="1"/>
+      <c r="H415" s="1"/>
+      <c r="I415" s="1"/>
+      <c r="J415" s="1"/>
+      <c r="K415" s="1"/>
+      <c r="L415" s="1"/>
+      <c r="M415" s="1"/>
+      <c r="N415" s="1"/>
+      <c r="O415" s="1"/>
+      <c r="P415" s="1"/>
+      <c r="Q415" s="1"/>
+      <c r="R415" s="1"/>
+      <c r="S415" s="1"/>
+      <c r="T415" s="1"/>
+      <c r="U415" s="1"/>
+      <c r="V415" s="1"/>
+      <c r="W415" s="1"/>
+      <c r="X415" s="1"/>
+      <c r="Y415" s="1"/>
+      <c r="Z415" s="1"/>
+      <c r="AA415" s="1"/>
+      <c r="AB415" s="1"/>
+      <c r="AC415" s="1"/>
+      <c r="AD415" s="1"/>
+      <c r="AE415" s="1"/>
+      <c r="AH415">
+        <f t="shared" ref="AH415:AI415" si="126">AH412</f>
+        <v>30</v>
+      </c>
+      <c r="AI415">
+        <f t="shared" si="126"/>
+        <v>0</v>
+      </c>
+      <c r="AT415">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW415" t="str">
+        <f t="shared" si="111"/>
+        <v>30,0</v>
+      </c>
+    </row>
+    <row r="416" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B416" s="1"/>
+      <c r="C416" s="1"/>
+      <c r="D416" s="1"/>
+      <c r="E416" s="1"/>
+      <c r="F416" s="1"/>
+      <c r="G416" s="1"/>
+      <c r="H416" s="1"/>
+      <c r="I416" s="1"/>
+      <c r="J416" s="1"/>
+      <c r="K416" s="1"/>
+      <c r="L416" s="1"/>
+      <c r="M416" s="1"/>
+      <c r="N416" s="1"/>
+      <c r="O416" s="1"/>
+      <c r="P416" s="1"/>
+      <c r="Q416" s="1"/>
+      <c r="R416" s="1"/>
+      <c r="S416" s="1"/>
+      <c r="T416" s="1"/>
+      <c r="U416" s="1"/>
+      <c r="V416" s="1"/>
+      <c r="W416" s="1"/>
+      <c r="X416" s="1"/>
+      <c r="Y416" s="1"/>
+      <c r="Z416" s="1"/>
+      <c r="AA416" s="1"/>
+      <c r="AB416" s="1"/>
+      <c r="AC416" s="1"/>
+      <c r="AD416" s="1"/>
+      <c r="AE416" s="1"/>
+      <c r="AH416">
+        <f t="shared" ref="AH416:AI416" si="127">AH413</f>
+        <v>30</v>
+      </c>
+      <c r="AI416">
+        <f t="shared" si="127"/>
+        <v>0</v>
+      </c>
+      <c r="AT416">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW416" t="str">
+        <f t="shared" si="111"/>
+        <v>30,0</v>
+      </c>
+    </row>
+    <row r="417" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B417" s="1"/>
+      <c r="C417" s="1"/>
+      <c r="D417" s="1"/>
+      <c r="E417" s="1"/>
+      <c r="F417" s="1"/>
+      <c r="G417" s="1"/>
+      <c r="H417" s="1"/>
+      <c r="I417" s="1"/>
+      <c r="J417" s="1">
+        <v>1</v>
+      </c>
+      <c r="K417" s="1">
+        <v>1</v>
+      </c>
+      <c r="L417" s="1">
+        <v>1</v>
+      </c>
+      <c r="M417" s="1">
+        <v>1</v>
+      </c>
+      <c r="N417" s="1">
+        <v>1</v>
+      </c>
+      <c r="O417" s="1">
+        <v>1</v>
+      </c>
+      <c r="P417" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q417" s="1">
+        <v>1</v>
+      </c>
+      <c r="R417" s="1">
+        <v>1</v>
+      </c>
+      <c r="S417" s="1">
+        <v>1</v>
+      </c>
+      <c r="T417" s="1">
+        <v>1</v>
+      </c>
+      <c r="U417" s="1">
+        <v>1</v>
+      </c>
+      <c r="V417" s="1">
+        <v>1</v>
+      </c>
+      <c r="W417" s="1">
+        <v>1</v>
+      </c>
+      <c r="X417" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y417" s="1"/>
+      <c r="Z417" s="1"/>
+      <c r="AA417" s="1"/>
+      <c r="AB417" s="1"/>
+      <c r="AC417" s="1"/>
+      <c r="AD417" s="1"/>
+      <c r="AE417" s="1"/>
+      <c r="AH417">
+        <f t="shared" ref="AH417:AK417" si="128">AH414</f>
+        <v>8</v>
+      </c>
+      <c r="AI417">
+        <f t="shared" si="128"/>
+        <v>15</v>
+      </c>
+      <c r="AJ417">
+        <f t="shared" si="128"/>
+        <v>7</v>
+      </c>
+      <c r="AK417">
+        <f t="shared" si="128"/>
+        <v>0</v>
+      </c>
+      <c r="AT417">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW417" t="str">
+        <f t="shared" si="111"/>
+        <v>8,15,7,0</v>
+      </c>
+    </row>
+    <row r="418" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="B418" s="1"/>
+      <c r="C418" s="1"/>
+      <c r="D418" s="1"/>
+      <c r="E418" s="1"/>
+      <c r="F418" s="1"/>
+      <c r="G418" s="1"/>
+      <c r="H418" s="1"/>
+      <c r="I418" s="1"/>
+      <c r="J418" s="1"/>
+      <c r="K418" s="1"/>
+      <c r="L418" s="1"/>
+      <c r="M418" s="1"/>
+      <c r="N418" s="1"/>
+      <c r="O418" s="1"/>
+      <c r="P418" s="1"/>
+      <c r="Q418" s="1"/>
+      <c r="R418" s="1"/>
+      <c r="S418" s="1"/>
+      <c r="T418" s="1"/>
+      <c r="U418" s="1"/>
+      <c r="V418" s="1"/>
+      <c r="W418" s="1"/>
+      <c r="X418" s="1"/>
+      <c r="Y418" s="1"/>
+      <c r="Z418" s="1"/>
+      <c r="AA418" s="1"/>
+      <c r="AB418" s="1"/>
+      <c r="AC418" s="1"/>
+      <c r="AD418" s="1"/>
+      <c r="AE418" s="1"/>
+      <c r="AH418">
+        <f t="shared" ref="AH418:AI418" si="129">AH415</f>
+        <v>30</v>
+      </c>
+      <c r="AI418">
+        <f t="shared" si="129"/>
+        <v>0</v>
+      </c>
+      <c r="AT418">
+        <f t="shared" si="110"/>
+        <v>30</v>
+      </c>
+      <c r="AW418" t="str">
+        <f t="shared" si="111"/>
+        <v>30,0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:AF97 AH14:AI14 AH31:AI31 G98:AF102 A98:E127 G103:T103 Z103:AF110 G104:X111 X111:AF111 G112:AF127 A128:AF143 A144:V159 AB144:AF159 A160:AF193 A194:A214 AF194:AF214 A215:AF215 A216:B216 C216:AF217 A217 A218:AF222 F222:X223 A223:J223 L223:AF223 AH243:AM243 AH244:AK246 AL245:AM245 AI246:AM246 AJ247:AK247 AH247:AH255 AI248:AK252 AL251:AM251 AI253:AJ253 AI254:AI255 A224:AF288 Q321 B291:AE319 A289:B289 AF289:AF321 A290:A321 AH305:AM305 AH347:AI347 A322:AF1048576">
+  <conditionalFormatting sqref="A1:AF97 AH14:AI14 AH31:AI31 G98:AF102 A98:E127 G103:T103 Z103:AF110 G104:X111 X111:AF111 G112:AF127 A128:AF143 A144:V159 AB144:AF159 A160:AF193 A194:A214 AF194:AF214 A215:AF215 A216:B216 C216:AF217 A217 A218:AF222 F222:X223 A223:J223 L223:AF223 A224:AF288 AH243:AM243 AH244:AK246 AL245:AM245 AI246:AM246 AJ247:AK247 AH247:AH255 AI248:AK252 AL251:AM251 AI253:AJ253 AI254:AI255 A289:B289 AF289:AF321 A290:A321 B291:AE319 Q321 AH347:AI347 A418:AF1048576 A322:AF404 A405:I417 Y405:AF417 B389:AE418">
     <cfRule type="cellIs" dxfId="7" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -34869,33 +36874,33 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C320:AE320">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AH46:AI46">
-    <cfRule type="cellIs" dxfId="5" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH258:AI266">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH269:AI277">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH305:AM306">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD46">
-    <cfRule type="cellIs" dxfId="2" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C320:AE320">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH306:AM306">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>